<commit_message>
Figure 3FG done 1. Figure 3FG script cleaned and comparmentalized 2. It also contains the binarized test script 3. Excel sheets added for the Figur3 F,G subpanels 4. Panel B script now also generates the innervation matrix
</commit_message>
<xml_diff>
--- a/data/Other/excelSheet/Fig3/Fig3BD_4BC.xlsx
+++ b/data/Other/excelSheet/Fig3/Fig3BD_4BC.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="71">
   <si>
     <t>treeIndex</t>
   </si>
@@ -258,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -286,11 +286,51 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -312,6 +352,46 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,36 +424,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="53" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -402,7 +482,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -431,7 +511,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="53" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -460,7 +540,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="53" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -489,7 +569,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="53" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -518,7 +598,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="53" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -547,7 +627,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="53" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -576,7 +656,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="53" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -605,7 +685,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="53" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -634,7 +714,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="53" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -663,7 +743,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="53" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -692,7 +772,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="53" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -721,7 +801,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="53" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -750,7 +830,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="53" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -779,7 +859,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="53" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -808,7 +888,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="53" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -837,7 +917,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="53" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -866,7 +946,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -895,7 +975,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="53" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -924,7 +1004,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="53" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -953,7 +1033,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -982,7 +1062,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="53" t="s">
         <v>50</v>
       </c>
       <c r="B23">
@@ -1011,7 +1091,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="53" t="s">
         <v>51</v>
       </c>
       <c r="B24">
@@ -1040,7 +1120,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="53" t="s">
         <v>52</v>
       </c>
       <c r="B25">
@@ -1069,7 +1149,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="53" t="s">
         <v>53</v>
       </c>
       <c r="B26">
@@ -1098,7 +1178,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="53" t="s">
         <v>54</v>
       </c>
       <c r="B27">
@@ -1127,7 +1207,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="53" t="s">
         <v>55</v>
       </c>
       <c r="B28">
@@ -1156,7 +1236,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="53" t="s">
         <v>56</v>
       </c>
       <c r="B29">
@@ -1185,7 +1265,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="53" t="s">
         <v>57</v>
       </c>
       <c r="B30">
@@ -1214,7 +1294,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="53" t="s">
         <v>58</v>
       </c>
       <c r="B31">
@@ -1263,36 +1343,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="55" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="55" t="s">
         <v>30</v>
       </c>
       <c r="B2">
@@ -1321,7 +1401,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="55" t="s">
         <v>31</v>
       </c>
       <c r="B3">
@@ -1350,7 +1430,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="55" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -1379,7 +1459,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="55" t="s">
         <v>33</v>
       </c>
       <c r="B5">
@@ -1408,7 +1488,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="55" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -1437,7 +1517,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="55" t="s">
         <v>35</v>
       </c>
       <c r="B7">
@@ -1466,7 +1546,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="55" t="s">
         <v>36</v>
       </c>
       <c r="B8">
@@ -1495,7 +1575,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="55" t="s">
         <v>37</v>
       </c>
       <c r="B9">
@@ -1524,7 +1604,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="55" t="s">
         <v>38</v>
       </c>
       <c r="B10">
@@ -1553,7 +1633,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="55" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -1582,7 +1662,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B12">
@@ -1611,7 +1691,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="55" t="s">
         <v>41</v>
       </c>
       <c r="B13">
@@ -1640,7 +1720,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="55" t="s">
         <v>42</v>
       </c>
       <c r="B14">
@@ -1669,7 +1749,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="55" t="s">
         <v>43</v>
       </c>
       <c r="B15">
@@ -1698,7 +1778,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="55" t="s">
         <v>44</v>
       </c>
       <c r="B16">
@@ -1727,7 +1807,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="55" t="s">
         <v>45</v>
       </c>
       <c r="B17">
@@ -1756,7 +1836,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="55" t="s">
         <v>46</v>
       </c>
       <c r="B18">
@@ -1785,7 +1865,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="55" t="s">
         <v>47</v>
       </c>
       <c r="B19">
@@ -1814,7 +1894,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="55" t="s">
         <v>48</v>
       </c>
       <c r="B20">
@@ -1843,7 +1923,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="55" t="s">
         <v>49</v>
       </c>
       <c r="B21">
@@ -1872,7 +1952,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="55" t="s">
         <v>59</v>
       </c>
       <c r="B22">
@@ -1901,7 +1981,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="55" t="s">
         <v>60</v>
       </c>
       <c r="B23">
@@ -1930,7 +2010,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="55" t="s">
         <v>61</v>
       </c>
       <c r="B24">
@@ -1959,7 +2039,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="55" t="s">
         <v>62</v>
       </c>
       <c r="B25">
@@ -1988,7 +2068,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="55" t="s">
         <v>63</v>
       </c>
       <c r="B26">
@@ -2017,7 +2097,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="55" t="s">
         <v>64</v>
       </c>
       <c r="B27">
@@ -2046,7 +2126,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="55" t="s">
         <v>65</v>
       </c>
       <c r="B28">
@@ -2075,7 +2155,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="55" t="s">
         <v>66</v>
       </c>
       <c r="B29">
@@ -2104,7 +2184,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="55" t="s">
         <v>67</v>
       </c>
       <c r="B30">
@@ -2133,7 +2213,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="55" t="s">
         <v>68</v>
       </c>
       <c r="B31">
@@ -2162,7 +2242,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="55" t="s">
         <v>69</v>
       </c>
       <c r="B32">
@@ -2191,7 +2271,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="55" t="s">
         <v>70</v>
       </c>
       <c r="B33">
@@ -2240,36 +2320,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="57" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -2298,7 +2378,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2327,7 +2407,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -2356,7 +2436,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -2385,7 +2465,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -2414,7 +2494,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -2443,7 +2523,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="57" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -2472,7 +2552,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="57" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -2501,7 +2581,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="57" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -2530,7 +2610,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -2559,7 +2639,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="57" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -2588,7 +2668,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -2617,7 +2697,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -2646,7 +2726,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="57" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -2675,7 +2755,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="57" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -2704,7 +2784,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -2733,7 +2813,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -2762,7 +2842,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -2791,7 +2871,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -2820,7 +2900,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -2849,7 +2929,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="57" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -2878,7 +2958,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B23">
@@ -2907,7 +2987,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B24">
@@ -2936,7 +3016,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B25">
@@ -2965,7 +3045,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B26">
@@ -2994,7 +3074,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B27">
@@ -3023,7 +3103,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B28">
@@ -3052,7 +3132,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="57" t="s">
         <v>7</v>
       </c>
       <c r="B29">
@@ -3081,7 +3161,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="57" t="s">
         <v>8</v>
       </c>
       <c r="B30">
@@ -3110,7 +3190,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="57" t="s">
         <v>9</v>
       </c>
       <c r="B31">
@@ -3139,7 +3219,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B32">
@@ -3168,7 +3248,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="57" t="s">
         <v>11</v>
       </c>
       <c r="B33">
@@ -3197,7 +3277,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B34">
@@ -3226,7 +3306,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B35">
@@ -3255,7 +3335,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="57" t="s">
         <v>14</v>
       </c>
       <c r="B36">
@@ -3284,7 +3364,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="57" t="s">
         <v>15</v>
       </c>
       <c r="B37">
@@ -3313,7 +3393,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B38">
@@ -3342,7 +3422,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B39">
@@ -3371,7 +3451,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B40">
@@ -3400,7 +3480,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B41">
@@ -3429,7 +3509,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B42">
@@ -3458,7 +3538,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B43">
@@ -3487,7 +3567,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B44">
@@ -3516,7 +3596,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B45">
@@ -3545,7 +3625,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B46">
@@ -3574,7 +3654,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B47">
@@ -3603,7 +3683,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B48">
@@ -3632,7 +3712,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="57" t="s">
         <v>7</v>
       </c>
       <c r="B49">
@@ -3661,7 +3741,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="57" t="s">
         <v>8</v>
       </c>
       <c r="B50">
@@ -3690,7 +3770,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="57" t="s">
         <v>9</v>
       </c>
       <c r="B51">
@@ -3719,7 +3799,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B52">
@@ -3748,7 +3828,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="57" t="s">
         <v>11</v>
       </c>
       <c r="B53">
@@ -3777,7 +3857,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B54">
@@ -3806,7 +3886,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B55">
@@ -3835,7 +3915,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="57" t="s">
         <v>14</v>
       </c>
       <c r="B56">
@@ -3864,7 +3944,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="57" t="s">
         <v>15</v>
       </c>
       <c r="B57">
@@ -3893,7 +3973,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B58">
@@ -3922,7 +4002,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B59">
@@ -3951,7 +4031,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B60">
@@ -3980,7 +4060,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B61">
@@ -4009,7 +4089,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B62">
@@ -4038,7 +4118,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="57" t="s">
         <v>21</v>
       </c>
       <c r="B63">
@@ -4067,7 +4147,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B64">
@@ -4096,7 +4176,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B65">
@@ -4125,7 +4205,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B66">
@@ -4154,7 +4234,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B67">
@@ -4183,7 +4263,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B68">
@@ -4212,7 +4292,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B69">
@@ -4241,7 +4321,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="57" t="s">
         <v>7</v>
       </c>
       <c r="B70">
@@ -4270,7 +4350,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="57" t="s">
         <v>8</v>
       </c>
       <c r="B71">
@@ -4299,7 +4379,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="57" t="s">
         <v>9</v>
       </c>
       <c r="B72">
@@ -4328,7 +4408,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B73">
@@ -4357,7 +4437,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="57" t="s">
         <v>11</v>
       </c>
       <c r="B74">
@@ -4386,7 +4466,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B75">
@@ -4415,7 +4495,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B76">
@@ -4444,7 +4524,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="57" t="s">
         <v>14</v>
       </c>
       <c r="B77">
@@ -4473,7 +4553,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="57" t="s">
         <v>15</v>
       </c>
       <c r="B78">
@@ -4502,7 +4582,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B79">
@@ -4531,7 +4611,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B80">
@@ -4560,7 +4640,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B81">
@@ -4589,7 +4669,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B82">
@@ -4618,7 +4698,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B83">
@@ -4647,7 +4727,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="17" t="s">
+      <c r="A84" s="57" t="s">
         <v>21</v>
       </c>
       <c r="B84">
@@ -4676,7 +4756,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="17" t="s">
+      <c r="A85" s="57" t="s">
         <v>50</v>
       </c>
       <c r="B85">
@@ -4705,7 +4785,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="57" t="s">
         <v>51</v>
       </c>
       <c r="B86">
@@ -4734,7 +4814,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="57" t="s">
         <v>52</v>
       </c>
       <c r="B87">
@@ -4763,7 +4843,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="17" t="s">
+      <c r="A88" s="57" t="s">
         <v>53</v>
       </c>
       <c r="B88">
@@ -4792,7 +4872,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="57" t="s">
         <v>54</v>
       </c>
       <c r="B89">
@@ -4821,7 +4901,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="57" t="s">
         <v>55</v>
       </c>
       <c r="B90">
@@ -4850,7 +4930,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="57" t="s">
         <v>56</v>
       </c>
       <c r="B91">
@@ -4879,7 +4959,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="57" t="s">
         <v>57</v>
       </c>
       <c r="B92">
@@ -4908,7 +4988,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="17" t="s">
+      <c r="A93" s="57" t="s">
         <v>58</v>
       </c>
       <c r="B93">
@@ -4957,36 +5037,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="59" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B2">
@@ -5015,7 +5095,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B3">
@@ -5044,7 +5124,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="59" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -5073,7 +5153,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B5">
@@ -5102,7 +5182,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="59" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -5131,7 +5211,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="59" t="s">
         <v>35</v>
       </c>
       <c r="B7">
@@ -5160,7 +5240,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B8">
@@ -5189,7 +5269,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="59" t="s">
         <v>37</v>
       </c>
       <c r="B9">
@@ -5218,7 +5298,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="59" t="s">
         <v>38</v>
       </c>
       <c r="B10">
@@ -5247,7 +5327,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -5276,7 +5356,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B12">
@@ -5305,7 +5385,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B13">
@@ -5334,7 +5414,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B14">
@@ -5363,7 +5443,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="59" t="s">
         <v>43</v>
       </c>
       <c r="B15">
@@ -5392,7 +5472,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B16">
@@ -5421,7 +5501,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B17">
@@ -5450,7 +5530,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="59" t="s">
         <v>46</v>
       </c>
       <c r="B18">
@@ -5479,7 +5559,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="59" t="s">
         <v>47</v>
       </c>
       <c r="B19">
@@ -5508,7 +5588,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="59" t="s">
         <v>48</v>
       </c>
       <c r="B20">
@@ -5537,7 +5617,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B21">
@@ -5566,7 +5646,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B22">
@@ -5595,7 +5675,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="59" t="s">
         <v>32</v>
       </c>
       <c r="B23">
@@ -5624,7 +5704,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B24">
@@ -5653,7 +5733,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="59" t="s">
         <v>34</v>
       </c>
       <c r="B25">
@@ -5682,7 +5762,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="59" t="s">
         <v>35</v>
       </c>
       <c r="B26">
@@ -5711,7 +5791,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B27">
@@ -5740,7 +5820,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="59" t="s">
         <v>37</v>
       </c>
       <c r="B28">
@@ -5769,7 +5849,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="59" t="s">
         <v>38</v>
       </c>
       <c r="B29">
@@ -5798,7 +5878,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B30">
@@ -5827,7 +5907,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B31">
@@ -5856,7 +5936,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B32">
@@ -5885,7 +5965,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B33">
@@ -5914,7 +5994,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="59" t="s">
         <v>43</v>
       </c>
       <c r="B34">
@@ -5943,7 +6023,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B35">
@@ -5972,7 +6052,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B36">
@@ -6001,7 +6081,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="59" t="s">
         <v>46</v>
       </c>
       <c r="B37">
@@ -6030,7 +6110,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="59" t="s">
         <v>47</v>
       </c>
       <c r="B38">
@@ -6059,7 +6139,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="59" t="s">
         <v>48</v>
       </c>
       <c r="B39">
@@ -6088,7 +6168,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="59" t="s">
         <v>49</v>
       </c>
       <c r="B40">
@@ -6117,7 +6197,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B41">
@@ -6146,7 +6226,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B42">
@@ -6175,7 +6255,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="59" t="s">
         <v>32</v>
       </c>
       <c r="B43">
@@ -6204,7 +6284,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B44">
@@ -6233,7 +6313,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="59" t="s">
         <v>34</v>
       </c>
       <c r="B45">
@@ -6262,7 +6342,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="59" t="s">
         <v>35</v>
       </c>
       <c r="B46">
@@ -6291,7 +6371,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B47">
@@ -6320,7 +6400,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="59" t="s">
         <v>37</v>
       </c>
       <c r="B48">
@@ -6349,7 +6429,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="59" t="s">
         <v>38</v>
       </c>
       <c r="B49">
@@ -6378,7 +6458,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B50">
@@ -6407,7 +6487,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B51">
@@ -6436,7 +6516,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B52">
@@ -6465,7 +6545,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B53">
@@ -6494,7 +6574,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="59" t="s">
         <v>43</v>
       </c>
       <c r="B54">
@@ -6523,7 +6603,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B55">
@@ -6552,7 +6632,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B56">
@@ -6581,7 +6661,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="59" t="s">
         <v>46</v>
       </c>
       <c r="B57">
@@ -6610,7 +6690,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="59" t="s">
         <v>47</v>
       </c>
       <c r="B58">
@@ -6639,7 +6719,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="59" t="s">
         <v>48</v>
       </c>
       <c r="B59">
@@ -6668,7 +6748,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="59" t="s">
         <v>49</v>
       </c>
       <c r="B60">
@@ -6697,7 +6777,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B61">
@@ -6726,7 +6806,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B62">
@@ -6755,7 +6835,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="59" t="s">
         <v>32</v>
       </c>
       <c r="B63">
@@ -6784,7 +6864,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B64">
@@ -6813,7 +6893,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="59" t="s">
         <v>34</v>
       </c>
       <c r="B65">
@@ -6842,7 +6922,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="59" t="s">
         <v>35</v>
       </c>
       <c r="B66">
@@ -6871,7 +6951,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B67">
@@ -6900,7 +6980,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="59" t="s">
         <v>37</v>
       </c>
       <c r="B68">
@@ -6929,7 +7009,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="59" t="s">
         <v>38</v>
       </c>
       <c r="B69">
@@ -6958,7 +7038,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B70">
@@ -6987,7 +7067,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B71">
@@ -7016,7 +7096,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B72">
@@ -7045,7 +7125,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B73">
@@ -7074,7 +7154,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="59" t="s">
         <v>43</v>
       </c>
       <c r="B74">
@@ -7103,7 +7183,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B75">
@@ -7132,7 +7212,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B76">
@@ -7161,7 +7241,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="59" t="s">
         <v>46</v>
       </c>
       <c r="B77">
@@ -7190,7 +7270,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="59" t="s">
         <v>47</v>
       </c>
       <c r="B78">
@@ -7219,7 +7299,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="59" t="s">
         <v>48</v>
       </c>
       <c r="B79">
@@ -7248,7 +7328,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="59" t="s">
         <v>49</v>
       </c>
       <c r="B80">
@@ -7277,7 +7357,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="19" t="s">
+      <c r="A81" s="59" t="s">
         <v>59</v>
       </c>
       <c r="B81">
@@ -7306,7 +7386,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="59" t="s">
         <v>60</v>
       </c>
       <c r="B82">
@@ -7335,7 +7415,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="59" t="s">
         <v>61</v>
       </c>
       <c r="B83">
@@ -7364,7 +7444,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="59" t="s">
         <v>62</v>
       </c>
       <c r="B84">
@@ -7393,7 +7473,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="59" t="s">
         <v>63</v>
       </c>
       <c r="B85">
@@ -7422,7 +7502,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="59" t="s">
         <v>64</v>
       </c>
       <c r="B86">
@@ -7451,7 +7531,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="19" t="s">
+      <c r="A87" s="59" t="s">
         <v>65</v>
       </c>
       <c r="B87">
@@ -7480,7 +7560,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="59" t="s">
         <v>66</v>
       </c>
       <c r="B88">
@@ -7509,7 +7589,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="19" t="s">
+      <c r="A89" s="59" t="s">
         <v>67</v>
       </c>
       <c r="B89">
@@ -7538,7 +7618,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="19" t="s">
+      <c r="A90" s="59" t="s">
         <v>68</v>
       </c>
       <c r="B90">
@@ -7567,7 +7647,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="19" t="s">
+      <c r="A91" s="59" t="s">
         <v>69</v>
       </c>
       <c r="B91">
@@ -7596,7 +7676,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="59" t="s">
         <v>70</v>
       </c>
       <c r="B92">
@@ -7661,36 +7741,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -7719,7 +7799,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -7748,7 +7828,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -7777,7 +7857,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -7806,7 +7886,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -7835,7 +7915,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -7864,7 +7944,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="41" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -7893,7 +7973,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -7922,7 +8002,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -7951,7 +8031,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -7980,7 +8060,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="41" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -8009,7 +8089,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -8038,7 +8118,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -8067,7 +8147,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -8096,7 +8176,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -8125,7 +8205,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -8154,7 +8234,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -8183,7 +8263,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -8212,7 +8292,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="41" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -8241,7 +8321,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="41" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -8270,7 +8350,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="41" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -8319,36 +8399,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="43" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="43" t="s">
         <v>30</v>
       </c>
       <c r="B2">
@@ -8377,7 +8457,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="43" t="s">
         <v>31</v>
       </c>
       <c r="B3">
@@ -8406,7 +8486,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="43" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -8435,7 +8515,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B5">
@@ -8464,7 +8544,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -8493,7 +8573,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="43" t="s">
         <v>35</v>
       </c>
       <c r="B7">
@@ -8522,7 +8602,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B8">
@@ -8551,7 +8631,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="43" t="s">
         <v>37</v>
       </c>
       <c r="B9">
@@ -8580,7 +8660,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="43" t="s">
         <v>38</v>
       </c>
       <c r="B10">
@@ -8609,7 +8689,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -8638,7 +8718,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="43" t="s">
         <v>40</v>
       </c>
       <c r="B12">
@@ -8667,7 +8747,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="43" t="s">
         <v>41</v>
       </c>
       <c r="B13">
@@ -8696,7 +8776,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B14">
@@ -8725,7 +8805,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B15">
@@ -8754,7 +8834,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="43" t="s">
         <v>44</v>
       </c>
       <c r="B16">
@@ -8783,7 +8863,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B17">
@@ -8812,7 +8892,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B18">
@@ -8841,7 +8921,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B19">
@@ -8870,7 +8950,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B20">
@@ -8919,36 +8999,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="45" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -8977,7 +9057,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -9006,7 +9086,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -9035,7 +9115,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -9064,7 +9144,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -9093,7 +9173,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -9122,7 +9202,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="45" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -9151,7 +9231,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -9180,7 +9260,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -9209,7 +9289,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -9238,7 +9318,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -9267,7 +9347,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -9296,7 +9376,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -9325,7 +9405,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -9354,7 +9434,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="45" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -9383,7 +9463,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="45" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -9412,7 +9492,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="45" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -9441,7 +9521,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="45" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -9470,7 +9550,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -9499,7 +9579,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="45" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -9548,36 +9628,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="47" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="47" t="s">
         <v>30</v>
       </c>
       <c r="B2">
@@ -9606,7 +9686,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="47" t="s">
         <v>31</v>
       </c>
       <c r="B3">
@@ -9635,7 +9715,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="47" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -9664,7 +9744,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
       <c r="B5">
@@ -9693,7 +9773,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="47" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -9722,7 +9802,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B7">
@@ -9751,7 +9831,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="47" t="s">
         <v>36</v>
       </c>
       <c r="B8">
@@ -9780,7 +9860,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B9">
@@ -9809,7 +9889,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B10">
@@ -9838,7 +9918,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="47" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -9867,7 +9947,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="47" t="s">
         <v>40</v>
       </c>
       <c r="B12">
@@ -9896,7 +9976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="47" t="s">
         <v>41</v>
       </c>
       <c r="B13">
@@ -9925,7 +10005,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B14">
@@ -9954,7 +10034,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="47" t="s">
         <v>43</v>
       </c>
       <c r="B15">
@@ -9983,7 +10063,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="47" t="s">
         <v>44</v>
       </c>
       <c r="B16">
@@ -10012,7 +10092,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B17">
@@ -10041,7 +10121,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="47" t="s">
         <v>46</v>
       </c>
       <c r="B18">
@@ -10070,7 +10150,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="47" t="s">
         <v>47</v>
       </c>
       <c r="B19">
@@ -10099,7 +10179,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="47" t="s">
         <v>48</v>
       </c>
       <c r="B20">
@@ -10128,7 +10208,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="47" t="s">
         <v>49</v>
       </c>
       <c r="B21">
@@ -10177,36 +10257,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="49" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="49" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -10235,7 +10315,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -10264,7 +10344,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -10293,7 +10373,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -10322,7 +10402,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -10351,7 +10431,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -10380,7 +10460,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -10409,7 +10489,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -10438,7 +10518,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -10467,7 +10547,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -10496,7 +10576,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="49" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -10525,7 +10605,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -10554,7 +10634,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="49" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -10583,7 +10663,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -10612,7 +10692,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="49" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -10641,7 +10721,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -10670,7 +10750,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -10699,7 +10779,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="49" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -10728,7 +10808,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -10757,7 +10837,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -10786,7 +10866,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="49" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -10835,36 +10915,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="51" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="51" t="s">
         <v>30</v>
       </c>
       <c r="B2">
@@ -10893,7 +10973,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B3">
@@ -10922,7 +11002,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="51" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -10951,7 +11031,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="51" t="s">
         <v>33</v>
       </c>
       <c r="B5">
@@ -10980,7 +11060,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="51" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -11009,7 +11089,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="51" t="s">
         <v>35</v>
       </c>
       <c r="B7">
@@ -11038,7 +11118,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="51" t="s">
         <v>36</v>
       </c>
       <c r="B8">
@@ -11067,7 +11147,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B9">
@@ -11096,7 +11176,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="51" t="s">
         <v>38</v>
       </c>
       <c r="B10">
@@ -11125,7 +11205,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="51" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -11154,7 +11234,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="51" t="s">
         <v>40</v>
       </c>
       <c r="B12">
@@ -11183,7 +11263,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="51" t="s">
         <v>41</v>
       </c>
       <c r="B13">
@@ -11212,7 +11292,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B14">
@@ -11241,7 +11321,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="51" t="s">
         <v>43</v>
       </c>
       <c r="B15">
@@ -11270,7 +11350,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="51" t="s">
         <v>44</v>
       </c>
       <c r="B16">
@@ -11299,7 +11379,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="51" t="s">
         <v>45</v>
       </c>
       <c r="B17">
@@ -11328,7 +11408,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="51" t="s">
         <v>46</v>
       </c>
       <c r="B18">
@@ -11357,7 +11437,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B19">
@@ -11386,7 +11466,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="51" t="s">
         <v>48</v>
       </c>
       <c r="B20">
@@ -11415,7 +11495,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="51" t="s">
         <v>49</v>
       </c>
       <c r="B21">

</xml_diff>